<commit_message>
Update CMS FOR LED 的调整（LEIVS）20190814.xlsx
</commit_message>
<xml_diff>
--- a/2019/武汉店/05 系统集成/LED信息/CMS FOR LED 的调整（LEIVS）20190814.xlsx
+++ b/2019/武汉店/05 系统集成/LED信息/CMS FOR LED 的调整（LEIVS）20190814.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="36" windowWidth="15960" windowHeight="7752"/>
+    <workbookView xWindow="7560" yWindow="36" windowWidth="15960" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="option 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="83">
   <si>
     <t>显示屏位置（mm）</t>
   </si>
@@ -282,34 +282,10 @@
     <t>1408*416</t>
   </si>
   <si>
-    <t>1080*1920</t>
-  </si>
-  <si>
-    <t>560*1920</t>
-  </si>
-  <si>
-    <t>1080*800</t>
-  </si>
-  <si>
-    <t>560*800</t>
-  </si>
-  <si>
     <t>1920*1080</t>
   </si>
   <si>
     <t>1920*440</t>
-  </si>
-  <si>
-    <t>1080*80</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1080*80</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>560*80</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>E1-5</t>
@@ -318,6 +294,12 @@
   <si>
     <t>E1-6</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1360*800</t>
+  </si>
+  <si>
+    <t>1360*400</t>
   </si>
 </sst>
 </file>
@@ -692,20 +674,75 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -716,62 +753,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1052,44 +1034,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>106681</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>144779</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1164859</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="图片 13"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13312141" y="9410699"/>
-          <a:ext cx="1058178" cy="1150621"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
       <xdr:colOff>350521</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>53341</xdr:rowOff>
@@ -1108,7 +1052,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1117,6 +1061,44 @@
         <a:xfrm>
           <a:off x="13555981" y="10736581"/>
           <a:ext cx="472439" cy="376435"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>41030</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1230923</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>136655</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13270522" y="9343293"/>
+          <a:ext cx="1189893" cy="998300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1138,14 +1120,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>98</xdr:col>
-      <xdr:colOff>476868</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>83674</xdr:rowOff>
+      <xdr:col>188</xdr:col>
+      <xdr:colOff>521136</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>57933</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="框架图.jpg"/>
+        <xdr:cNvPr id="4" name="框架图.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1161,7 +1143,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="60217668" cy="10690714"/>
+          <a:ext cx="115125936" cy="17759193"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2255,8 +2237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IP51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2553,60 +2535,60 @@
       <c r="M19" s="7"/>
     </row>
     <row r="20" spans="1:13" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="43" t="s">
+      <c r="B20" s="47"/>
+      <c r="C20" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="44"/>
-      <c r="F20" s="33" t="s">
+      <c r="E20" s="51"/>
+      <c r="F20" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="H20" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="49" t="s">
+      <c r="J20" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="K20" s="33" t="s">
+      <c r="K20" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="L20" s="33" t="s">
+      <c r="L20" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="M20" s="33" t="s">
+      <c r="M20" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="47"/>
+      <c r="A21" s="48"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="54"/>
       <c r="D21" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
     </row>
     <row r="22" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
@@ -2641,7 +2623,7 @@
       </c>
       <c r="K22" s="11"/>
       <c r="L22" s="27"/>
-      <c r="M22" s="38"/>
+      <c r="M22" s="37"/>
     </row>
     <row r="23" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
@@ -2653,32 +2635,32 @@
       <c r="C23" s="11">
         <v>1</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="52" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="45">
+      <c r="F23" s="33">
         <v>5</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23" s="34">
         <v>5</v>
       </c>
-      <c r="H23" s="45">
+      <c r="H23" s="33">
         <v>5</v>
       </c>
-      <c r="I23" s="45">
+      <c r="I23" s="33">
         <v>5</v>
       </c>
       <c r="J23" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="K23" s="45"/>
-      <c r="L23" s="54" t="s">
+      <c r="K23" s="33"/>
+      <c r="L23" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M23" s="38"/>
+      <c r="M23" s="37"/>
     </row>
     <row r="24" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
@@ -2690,20 +2672,20 @@
       <c r="C24" s="11">
         <v>1</v>
       </c>
-      <c r="D24" s="30"/>
+      <c r="D24" s="35"/>
       <c r="E24" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="45"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
       <c r="J24" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="K24" s="38"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="38"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="37"/>
     </row>
     <row r="25" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
@@ -2721,16 +2703,16 @@
       <c r="E25" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="F25" s="45"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
       <c r="J25" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="K25" s="38"/>
-      <c r="L25" s="53"/>
-      <c r="M25" s="38"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="37"/>
     </row>
     <row r="26" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
@@ -2742,22 +2724,22 @@
       <c r="C26" s="11">
         <v>1</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="52" t="s">
         <v>56</v>
       </c>
       <c r="E26" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="45"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
       <c r="J26" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="K26" s="38"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="38"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="37"/>
     </row>
     <row r="27" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
@@ -2769,20 +2751,20 @@
       <c r="C27" s="11">
         <v>1</v>
       </c>
-      <c r="D27" s="30"/>
+      <c r="D27" s="35"/>
       <c r="E27" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="F27" s="45"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
       <c r="J27" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="K27" s="38"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="38"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="37"/>
     </row>
     <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
@@ -2794,32 +2776,32 @@
       <c r="C28" s="23">
         <v>1</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="52" t="s">
         <v>55</v>
       </c>
       <c r="E28" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F28" s="29">
+      <c r="F28" s="34">
         <v>3</v>
       </c>
-      <c r="G28" s="29">
+      <c r="G28" s="34">
         <v>3</v>
       </c>
-      <c r="H28" s="29">
+      <c r="H28" s="34">
         <v>3</v>
       </c>
-      <c r="I28" s="29">
+      <c r="I28" s="34">
         <v>3</v>
       </c>
       <c r="J28" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="K28" s="48"/>
-      <c r="L28" s="54" t="s">
+      <c r="K28" s="36"/>
+      <c r="L28" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="M28" s="38"/>
+      <c r="M28" s="37"/>
     </row>
     <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
@@ -2831,20 +2813,20 @@
       <c r="C29" s="23">
         <v>1</v>
       </c>
-      <c r="D29" s="37"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="37"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
       <c r="J29" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="K29" s="38"/>
-      <c r="L29" s="53"/>
-      <c r="M29" s="38"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="37"/>
     </row>
     <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
@@ -2856,20 +2838,20 @@
       <c r="C30" s="23">
         <v>1</v>
       </c>
-      <c r="D30" s="38"/>
+      <c r="D30" s="37"/>
       <c r="E30" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="F30" s="38"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
       <c r="J30" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="K30" s="38"/>
-      <c r="L30" s="53"/>
-      <c r="M30" s="38"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="37"/>
     </row>
     <row r="31" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
@@ -2881,22 +2863,22 @@
       <c r="C31" s="11">
         <v>1</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="52" t="s">
         <v>51</v>
       </c>
       <c r="E31" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="F31" s="29">
+      <c r="F31" s="34">
         <v>3</v>
       </c>
-      <c r="G31" s="29">
+      <c r="G31" s="34">
         <v>3</v>
       </c>
-      <c r="H31" s="29">
+      <c r="H31" s="34">
         <v>3</v>
       </c>
-      <c r="I31" s="29">
+      <c r="I31" s="34">
         <v>3</v>
       </c>
       <c r="J31" s="21" t="s">
@@ -2904,7 +2886,7 @@
       </c>
       <c r="K31" s="12"/>
       <c r="L31" s="27"/>
-      <c r="M31" s="38"/>
+      <c r="M31" s="37"/>
     </row>
     <row r="32" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
@@ -2916,20 +2898,20 @@
       <c r="C32" s="11">
         <v>1</v>
       </c>
-      <c r="D32" s="32"/>
+      <c r="D32" s="38"/>
       <c r="E32" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
       <c r="J32" s="21" t="s">
         <v>70</v>
       </c>
       <c r="K32" s="12"/>
       <c r="L32" s="27"/>
-      <c r="M32" s="38"/>
+      <c r="M32" s="37"/>
     </row>
     <row r="33" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
@@ -2941,20 +2923,20 @@
       <c r="C33" s="11">
         <v>1</v>
       </c>
-      <c r="D33" s="30"/>
+      <c r="D33" s="35"/>
       <c r="E33" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
       <c r="J33" s="21" t="s">
         <v>71</v>
       </c>
       <c r="K33" s="12"/>
       <c r="L33" s="27"/>
-      <c r="M33" s="38"/>
+      <c r="M33" s="37"/>
     </row>
     <row r="34" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
@@ -2966,32 +2948,32 @@
       <c r="C34" s="11">
         <v>1</v>
       </c>
-      <c r="D34" s="31" t="s">
+      <c r="D34" s="52" t="s">
         <v>52</v>
       </c>
       <c r="E34" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F34" s="45">
+      <c r="F34" s="33">
         <v>4</v>
       </c>
-      <c r="G34" s="29">
+      <c r="G34" s="34">
         <v>4</v>
       </c>
-      <c r="H34" s="45">
+      <c r="H34" s="33">
         <v>4</v>
       </c>
-      <c r="I34" s="45">
+      <c r="I34" s="33">
         <v>4</v>
       </c>
       <c r="J34" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="K34" s="48"/>
-      <c r="L34" s="54" t="s">
+      <c r="K34" s="36"/>
+      <c r="L34" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M34" s="38"/>
+      <c r="M34" s="37"/>
     </row>
     <row r="35" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
@@ -3003,20 +2985,20 @@
       <c r="C35" s="11">
         <v>1</v>
       </c>
-      <c r="D35" s="30"/>
+      <c r="D35" s="35"/>
       <c r="E35" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F35" s="45"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="45"/>
-      <c r="I35" s="45"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
       <c r="J35" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="K35" s="38"/>
-      <c r="L35" s="53"/>
-      <c r="M35" s="38"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="40"/>
+      <c r="M35" s="37"/>
     </row>
     <row r="36" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
@@ -3034,16 +3016,16 @@
       <c r="E36" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="F36" s="45"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
       <c r="J36" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="K36" s="38"/>
-      <c r="L36" s="53"/>
-      <c r="M36" s="38"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="37"/>
     </row>
     <row r="37" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -3061,16 +3043,16 @@
       <c r="E37" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F37" s="45"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
       <c r="J37" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="K37" s="38"/>
-      <c r="L37" s="53"/>
-      <c r="M37" s="38"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="40"/>
+      <c r="M37" s="37"/>
     </row>
     <row r="38" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="20" t="s">
@@ -3082,22 +3064,22 @@
       <c r="C38" s="22">
         <v>1</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="56" t="s">
         <v>60</v>
       </c>
       <c r="E38" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="F38" s="29">
+      <c r="F38" s="34">
         <v>2</v>
       </c>
-      <c r="G38" s="29">
+      <c r="G38" s="34">
         <v>2</v>
       </c>
-      <c r="H38" s="29">
+      <c r="H38" s="34">
         <v>2</v>
       </c>
-      <c r="I38" s="29">
+      <c r="I38" s="34">
         <v>2</v>
       </c>
       <c r="J38" s="21" t="s">
@@ -3105,7 +3087,7 @@
       </c>
       <c r="K38" s="12"/>
       <c r="L38" s="27"/>
-      <c r="M38" s="38"/>
+      <c r="M38" s="37"/>
     </row>
     <row r="39" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="20" t="s">
@@ -3117,20 +3099,20 @@
       <c r="C39" s="22">
         <v>1</v>
       </c>
-      <c r="D39" s="36"/>
+      <c r="D39" s="57"/>
       <c r="E39" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="35"/>
       <c r="J39" s="21" t="s">
         <v>76</v>
       </c>
       <c r="K39" s="12"/>
       <c r="L39" s="27"/>
-      <c r="M39" s="38"/>
+      <c r="M39" s="37"/>
     </row>
     <row r="40" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
@@ -3165,7 +3147,7 @@
       </c>
       <c r="K40" s="12"/>
       <c r="L40" s="27"/>
-      <c r="M40" s="38"/>
+      <c r="M40" s="37"/>
     </row>
     <row r="41" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
@@ -3200,7 +3182,7 @@
       </c>
       <c r="K41" s="12"/>
       <c r="L41" s="27"/>
-      <c r="M41" s="38"/>
+      <c r="M41" s="37"/>
     </row>
     <row r="42" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
@@ -3235,7 +3217,7 @@
       </c>
       <c r="K42" s="12"/>
       <c r="L42" s="27"/>
-      <c r="M42" s="38"/>
+      <c r="M42" s="37"/>
     </row>
     <row r="43" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
@@ -3247,30 +3229,30 @@
       <c r="C43" s="11">
         <v>1</v>
       </c>
-      <c r="D43" s="35" t="s">
+      <c r="D43" s="56" t="s">
         <v>61</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="F43" s="56">
+        <v>81</v>
+      </c>
+      <c r="F43" s="41">
         <v>6</v>
       </c>
-      <c r="G43" s="56">
+      <c r="G43" s="41">
         <v>6</v>
       </c>
-      <c r="H43" s="56">
+      <c r="H43" s="41">
         <v>6</v>
       </c>
-      <c r="I43" s="56">
+      <c r="I43" s="41">
         <v>6</v>
       </c>
       <c r="J43" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="K43" s="48"/>
-      <c r="L43" s="53"/>
-      <c r="M43" s="38"/>
+        <v>81</v>
+      </c>
+      <c r="K43" s="36"/>
+      <c r="L43" s="40"/>
+      <c r="M43" s="37"/>
     </row>
     <row r="44" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
@@ -3282,20 +3264,20 @@
       <c r="C44" s="23">
         <v>1</v>
       </c>
-      <c r="D44" s="57"/>
+      <c r="D44" s="58"/>
       <c r="E44" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="F44" s="58"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
+        <v>81</v>
+      </c>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
       <c r="J44" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="K44" s="48"/>
-      <c r="L44" s="53"/>
-      <c r="M44" s="38"/>
+        <v>81</v>
+      </c>
+      <c r="K44" s="36"/>
+      <c r="L44" s="40"/>
+      <c r="M44" s="37"/>
     </row>
     <row r="45" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
@@ -3307,20 +3289,20 @@
       <c r="C45" s="23">
         <v>1</v>
       </c>
-      <c r="D45" s="57"/>
+      <c r="D45" s="58"/>
       <c r="E45" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F45" s="58"/>
-      <c r="G45" s="58"/>
-      <c r="H45" s="58"/>
-      <c r="I45" s="58"/>
+        <v>81</v>
+      </c>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="42"/>
       <c r="J45" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="K45" s="48"/>
-      <c r="L45" s="53"/>
-      <c r="M45" s="38"/>
+        <v>81</v>
+      </c>
+      <c r="K45" s="36"/>
+      <c r="L45" s="40"/>
+      <c r="M45" s="37"/>
     </row>
     <row r="46" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
@@ -3332,70 +3314,70 @@
       <c r="C46" s="28">
         <v>1</v>
       </c>
-      <c r="D46" s="57"/>
+      <c r="D46" s="58"/>
       <c r="E46" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F46" s="58"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="58"/>
+        <v>81</v>
+      </c>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="42"/>
       <c r="J46" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="K46" s="48"/>
-      <c r="L46" s="53"/>
-      <c r="M46" s="38"/>
+        <v>81</v>
+      </c>
+      <c r="K46" s="36"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="37"/>
     </row>
     <row r="47" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
         <v>36</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C47" s="28">
         <v>1</v>
       </c>
-      <c r="D47" s="57"/>
+      <c r="D47" s="58"/>
       <c r="E47" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="58"/>
-      <c r="I47" s="58"/>
+        <v>82</v>
+      </c>
+      <c r="F47" s="42"/>
+      <c r="G47" s="42"/>
+      <c r="H47" s="42"/>
+      <c r="I47" s="42"/>
       <c r="J47" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="K47" s="48"/>
-      <c r="L47" s="53"/>
-      <c r="M47" s="38"/>
+        <v>82</v>
+      </c>
+      <c r="K47" s="36"/>
+      <c r="L47" s="40"/>
+      <c r="M47" s="37"/>
     </row>
     <row r="48" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C48" s="11">
         <v>1</v>
       </c>
-      <c r="D48" s="58"/>
+      <c r="D48" s="42"/>
       <c r="E48" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="F48" s="58"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="58"/>
+        <v>82</v>
+      </c>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="42"/>
       <c r="J48" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="K48" s="38"/>
-      <c r="L48" s="53"/>
-      <c r="M48" s="38"/>
+        <v>82</v>
+      </c>
+      <c r="K48" s="37"/>
+      <c r="L48" s="40"/>
+      <c r="M48" s="37"/>
     </row>
     <row r="49" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
@@ -3407,30 +3389,30 @@
       <c r="C49" s="11">
         <v>1</v>
       </c>
-      <c r="D49" s="31" t="s">
+      <c r="D49" s="52" t="s">
         <v>54</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F49" s="29">
+        <v>77</v>
+      </c>
+      <c r="F49" s="34">
         <v>2</v>
       </c>
-      <c r="G49" s="29">
+      <c r="G49" s="34">
         <v>2</v>
       </c>
-      <c r="H49" s="29">
+      <c r="H49" s="34">
         <v>2</v>
       </c>
-      <c r="I49" s="29">
+      <c r="I49" s="34">
         <v>2</v>
       </c>
       <c r="J49" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="K49" s="48"/>
-      <c r="L49" s="51"/>
-      <c r="M49" s="38"/>
+        <v>77</v>
+      </c>
+      <c r="K49" s="36"/>
+      <c r="L49" s="44"/>
+      <c r="M49" s="37"/>
     </row>
     <row r="50" spans="1:13" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
@@ -3442,20 +3424,20 @@
       <c r="C50" s="11">
         <v>1</v>
       </c>
-      <c r="D50" s="30"/>
+      <c r="D50" s="35"/>
       <c r="E50" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="F50" s="30"/>
-      <c r="G50" s="30"/>
-      <c r="H50" s="30"/>
-      <c r="I50" s="30"/>
+        <v>78</v>
+      </c>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
       <c r="J50" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="K50" s="38"/>
-      <c r="L50" s="52"/>
-      <c r="M50" s="38"/>
+        <v>78</v>
+      </c>
+      <c r="K50" s="37"/>
+      <c r="L50" s="45"/>
+      <c r="M50" s="37"/>
     </row>
     <row r="51" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="13"/>
@@ -3488,18 +3470,35 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="I23:I27"/>
-    <mergeCell ref="I49:I50"/>
-    <mergeCell ref="H23:H27"/>
-    <mergeCell ref="K34:K37"/>
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="L34:L37"/>
-    <mergeCell ref="I34:I37"/>
-    <mergeCell ref="L23:L27"/>
-    <mergeCell ref="I43:I48"/>
-    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="H43:H48"/>
+    <mergeCell ref="F43:F48"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="D43:D48"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="G28:G30"/>
     <mergeCell ref="M20:M50"/>
     <mergeCell ref="K28:K30"/>
     <mergeCell ref="I31:I33"/>
@@ -3516,35 +3515,18 @@
     <mergeCell ref="K43:K48"/>
     <mergeCell ref="K23:K27"/>
     <mergeCell ref="I28:I30"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="F23:F27"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="G28:G30"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="H43:H48"/>
-    <mergeCell ref="F43:F48"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="D43:D48"/>
+    <mergeCell ref="L34:L37"/>
+    <mergeCell ref="I34:I37"/>
+    <mergeCell ref="L23:L27"/>
+    <mergeCell ref="I43:I48"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="I23:I27"/>
+    <mergeCell ref="I49:I50"/>
+    <mergeCell ref="H23:H27"/>
+    <mergeCell ref="K34:K37"/>
+    <mergeCell ref="H31:H33"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3560,7 +3542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="BC1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
+    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>